<commit_message>
testing here and there
</commit_message>
<xml_diff>
--- a/excelFiles/Справочник_ФЛК_УПДТ.xlsx
+++ b/excelFiles/Справочник_ФЛК_УПДТ.xlsx
@@ -912,71 +912,218 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -989,153 +1136,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1489,7 +1489,7 @@
   <dimension ref="A1:J489"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,7 +1631,7 @@
       </c>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>6730</v>
       </c>
@@ -6844,302 +6844,302 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="76"/>
-      <c r="U1" s="76"/>
-      <c r="V1" s="76"/>
-      <c r="W1" s="76"/>
-      <c r="X1" s="76"/>
-      <c r="Y1" s="76"/>
-      <c r="Z1" s="76"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="79"/>
+      <c r="X1" s="79"/>
+      <c r="Y1" s="79"/>
+      <c r="Z1" s="79"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
-      <c r="P2" s="76"/>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="76"/>
-      <c r="S2" s="76"/>
-      <c r="T2" s="76"/>
-      <c r="U2" s="76"/>
-      <c r="V2" s="76"/>
-      <c r="W2" s="76"/>
-      <c r="X2" s="76"/>
-      <c r="Y2" s="76"/>
-      <c r="Z2" s="76"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="79"/>
+      <c r="Q2" s="79"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="79"/>
+      <c r="U2" s="79"/>
+      <c r="V2" s="79"/>
+      <c r="W2" s="79"/>
+      <c r="X2" s="79"/>
+      <c r="Y2" s="79"/>
+      <c r="Z2" s="79"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="43"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="43"/>
-      <c r="W3" s="43"/>
-      <c r="X3" s="43"/>
-      <c r="Y3" s="43"/>
-      <c r="Z3" s="40"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="39"/>
       <c r="AA3" s="22"/>
       <c r="AB3" s="22"/>
     </row>
     <row r="4" spans="1:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="30" t="s">
+      <c r="B4" s="93"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="36" t="s">
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="39" t="s">
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
+      <c r="M4" s="98"/>
+      <c r="N4" s="98"/>
+      <c r="O4" s="98"/>
+      <c r="P4" s="98"/>
+      <c r="Q4" s="98"/>
+      <c r="R4" s="98"/>
+      <c r="S4" s="84"/>
+      <c r="T4" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
-      <c r="W4" s="43"/>
-      <c r="X4" s="40"/>
-      <c r="Y4" s="39" t="s">
+      <c r="U4" s="38"/>
+      <c r="V4" s="38"/>
+      <c r="W4" s="38"/>
+      <c r="X4" s="39"/>
+      <c r="Y4" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Z4" s="40"/>
+      <c r="Z4" s="39"/>
       <c r="AA4" s="22"/>
       <c r="AB4" s="23"/>
     </row>
     <row r="5" spans="1:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="33"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="36" t="s">
+      <c r="A5" s="77"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="39" t="s">
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="98"/>
+      <c r="Q5" s="98"/>
+      <c r="R5" s="98"/>
+      <c r="S5" s="84"/>
+      <c r="T5" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="U5" s="43"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="43"/>
-      <c r="X5" s="40"/>
-      <c r="Y5" s="39" t="s">
+      <c r="U5" s="38"/>
+      <c r="V5" s="38"/>
+      <c r="W5" s="38"/>
+      <c r="X5" s="39"/>
+      <c r="Y5" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Z5" s="40"/>
+      <c r="Z5" s="39"/>
       <c r="AA5" s="22"/>
       <c r="AB5" s="23"/>
     </row>
     <row r="6" spans="1:28" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="39" t="s">
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="43"/>
-      <c r="S6" s="43"/>
-      <c r="T6" s="40"/>
-      <c r="U6" s="39" t="s">
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="38"/>
+      <c r="T6" s="39"/>
+      <c r="U6" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="V6" s="43"/>
-      <c r="W6" s="43"/>
-      <c r="X6" s="40"/>
-      <c r="Y6" s="39" t="s">
+      <c r="V6" s="38"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="39"/>
+      <c r="Y6" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="Z6" s="40"/>
+      <c r="Z6" s="39"/>
       <c r="AA6" s="24"/>
       <c r="AB6" s="24"/>
     </row>
     <row r="7" spans="1:28" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="44" t="s">
+      <c r="F7" s="60"/>
+      <c r="G7" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="45"/>
-      <c r="I7" s="41" t="s">
+      <c r="H7" s="60"/>
+      <c r="I7" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="41" t="s">
+      <c r="J7" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="41" t="s">
+      <c r="K7" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="39" t="s">
+      <c r="L7" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="40"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="39"/>
       <c r="Q7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="R7" s="39" t="s">
+      <c r="R7" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="S7" s="43"/>
-      <c r="T7" s="40"/>
-      <c r="U7" s="39" t="s">
+      <c r="S7" s="38"/>
+      <c r="T7" s="39"/>
+      <c r="U7" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="V7" s="40"/>
-      <c r="W7" s="39" t="s">
+      <c r="V7" s="39"/>
+      <c r="W7" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="X7" s="40"/>
-      <c r="Y7" s="36"/>
-      <c r="Z7" s="38"/>
-      <c r="AA7" s="51"/>
-      <c r="AB7" s="52"/>
+      <c r="X7" s="39"/>
+      <c r="Y7" s="83"/>
+      <c r="Z7" s="84"/>
+      <c r="AA7" s="85"/>
+      <c r="AB7" s="101"/>
     </row>
     <row r="8" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="42"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="39" t="s">
+      <c r="A8" s="97"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="97"/>
+      <c r="J8" s="97"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="M8" s="43"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="39" t="s">
+      <c r="M8" s="38"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="P8" s="40"/>
+      <c r="P8" s="39"/>
       <c r="Q8" s="12"/>
-      <c r="R8" s="53"/>
-      <c r="S8" s="54"/>
-      <c r="T8" s="55"/>
-      <c r="U8" s="53"/>
-      <c r="V8" s="55"/>
-      <c r="W8" s="53"/>
-      <c r="X8" s="55"/>
-      <c r="Y8" s="56"/>
-      <c r="Z8" s="57"/>
-      <c r="AA8" s="51"/>
-      <c r="AB8" s="60"/>
+      <c r="R8" s="102"/>
+      <c r="S8" s="103"/>
+      <c r="T8" s="104"/>
+      <c r="U8" s="102"/>
+      <c r="V8" s="104"/>
+      <c r="W8" s="102"/>
+      <c r="X8" s="104"/>
+      <c r="Y8" s="87"/>
+      <c r="Z8" s="89"/>
+      <c r="AA8" s="85"/>
+      <c r="AB8" s="86"/>
     </row>
     <row r="9" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
@@ -7154,14 +7154,14 @@
       <c r="D9" s="14">
         <v>704</v>
       </c>
-      <c r="E9" s="48">
+      <c r="E9" s="40">
         <v>705</v>
       </c>
-      <c r="F9" s="49"/>
-      <c r="G9" s="48">
+      <c r="F9" s="42"/>
+      <c r="G9" s="40">
         <v>806</v>
       </c>
-      <c r="H9" s="49"/>
+      <c r="H9" s="42"/>
       <c r="I9" s="14">
         <v>807</v>
       </c>
@@ -7171,619 +7171,619 @@
       <c r="K9" s="14">
         <v>809</v>
       </c>
-      <c r="L9" s="48">
+      <c r="L9" s="40">
         <v>810</v>
       </c>
-      <c r="M9" s="50"/>
-      <c r="N9" s="49"/>
-      <c r="O9" s="48">
+      <c r="M9" s="41"/>
+      <c r="N9" s="42"/>
+      <c r="O9" s="40">
         <v>811</v>
       </c>
-      <c r="P9" s="49"/>
+      <c r="P9" s="42"/>
       <c r="Q9" s="14">
         <v>812</v>
       </c>
-      <c r="R9" s="48">
+      <c r="R9" s="40">
         <v>813</v>
       </c>
-      <c r="S9" s="50"/>
-      <c r="T9" s="49"/>
-      <c r="U9" s="48">
+      <c r="S9" s="41"/>
+      <c r="T9" s="42"/>
+      <c r="U9" s="40">
         <v>914</v>
       </c>
-      <c r="V9" s="49"/>
-      <c r="W9" s="48">
+      <c r="V9" s="42"/>
+      <c r="W9" s="40">
         <v>915</v>
       </c>
-      <c r="X9" s="49"/>
-      <c r="Y9" s="58"/>
-      <c r="Z9" s="59"/>
-      <c r="AA9" s="51"/>
-      <c r="AB9" s="60"/>
+      <c r="X9" s="42"/>
+      <c r="Y9" s="90"/>
+      <c r="Z9" s="92"/>
+      <c r="AA9" s="85"/>
+      <c r="AB9" s="86"/>
     </row>
     <row r="10" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="41">
+      <c r="A10" s="95">
         <v>1</v>
       </c>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="64" t="s">
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="65"/>
+      <c r="H10" s="100"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="38"/>
+      <c r="L10" s="83"/>
+      <c r="M10" s="98"/>
+      <c r="N10" s="84"/>
+      <c r="O10" s="83"/>
+      <c r="P10" s="84"/>
       <c r="Q10" s="15"/>
-      <c r="R10" s="36"/>
-      <c r="S10" s="37"/>
-      <c r="T10" s="38"/>
-      <c r="U10" s="36"/>
-      <c r="V10" s="38"/>
-      <c r="W10" s="36"/>
-      <c r="X10" s="38"/>
-      <c r="Y10" s="36"/>
-      <c r="Z10" s="38"/>
-      <c r="AA10" s="51"/>
-      <c r="AB10" s="60"/>
+      <c r="R10" s="83"/>
+      <c r="S10" s="98"/>
+      <c r="T10" s="84"/>
+      <c r="U10" s="83"/>
+      <c r="V10" s="84"/>
+      <c r="W10" s="83"/>
+      <c r="X10" s="84"/>
+      <c r="Y10" s="83"/>
+      <c r="Z10" s="84"/>
+      <c r="AA10" s="85"/>
+      <c r="AB10" s="86"/>
     </row>
     <row r="11" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="61"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="64" t="s">
+      <c r="A11" s="96"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="H11" s="65"/>
+      <c r="H11" s="100"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="36"/>
-      <c r="P11" s="38"/>
+      <c r="L11" s="83"/>
+      <c r="M11" s="98"/>
+      <c r="N11" s="84"/>
+      <c r="O11" s="83"/>
+      <c r="P11" s="84"/>
       <c r="Q11" s="15"/>
-      <c r="R11" s="36"/>
-      <c r="S11" s="37"/>
-      <c r="T11" s="38"/>
-      <c r="U11" s="36"/>
-      <c r="V11" s="38"/>
-      <c r="W11" s="36"/>
-      <c r="X11" s="38"/>
-      <c r="Y11" s="36"/>
-      <c r="Z11" s="38"/>
-      <c r="AA11" s="51"/>
-      <c r="AB11" s="60"/>
+      <c r="R11" s="83"/>
+      <c r="S11" s="98"/>
+      <c r="T11" s="84"/>
+      <c r="U11" s="83"/>
+      <c r="V11" s="84"/>
+      <c r="W11" s="83"/>
+      <c r="X11" s="84"/>
+      <c r="Y11" s="83"/>
+      <c r="Z11" s="84"/>
+      <c r="AA11" s="85"/>
+      <c r="AB11" s="86"/>
     </row>
     <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="61"/>
-      <c r="B12" s="68" t="s">
+      <c r="A12" s="96"/>
+      <c r="B12" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="70"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="45"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="60"/>
       <c r="Q12" s="21"/>
-      <c r="R12" s="44"/>
-      <c r="S12" s="66"/>
-      <c r="T12" s="45"/>
-      <c r="U12" s="30"/>
-      <c r="V12" s="31"/>
-      <c r="W12" s="31"/>
-      <c r="X12" s="31"/>
-      <c r="Y12" s="31"/>
-      <c r="Z12" s="32"/>
-      <c r="AA12" s="51"/>
-      <c r="AB12" s="60"/>
+      <c r="R12" s="58"/>
+      <c r="S12" s="59"/>
+      <c r="T12" s="60"/>
+      <c r="U12" s="75"/>
+      <c r="V12" s="93"/>
+      <c r="W12" s="93"/>
+      <c r="X12" s="93"/>
+      <c r="Y12" s="93"/>
+      <c r="Z12" s="76"/>
+      <c r="AA12" s="85"/>
+      <c r="AB12" s="86"/>
     </row>
     <row r="13" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="42"/>
-      <c r="B13" s="77" t="s">
+      <c r="A13" s="97"/>
+      <c r="B13" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="78"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="67"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="47"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="64"/>
+      <c r="M13" s="65"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="64"/>
+      <c r="P13" s="66"/>
       <c r="Q13" s="9"/>
-      <c r="R13" s="46"/>
-      <c r="S13" s="67"/>
-      <c r="T13" s="47"/>
-      <c r="U13" s="33"/>
-      <c r="V13" s="34"/>
-      <c r="W13" s="34"/>
-      <c r="X13" s="34"/>
-      <c r="Y13" s="34"/>
-      <c r="Z13" s="35"/>
-      <c r="AA13" s="51"/>
-      <c r="AB13" s="60"/>
+      <c r="R13" s="64"/>
+      <c r="S13" s="65"/>
+      <c r="T13" s="66"/>
+      <c r="U13" s="77"/>
+      <c r="V13" s="94"/>
+      <c r="W13" s="94"/>
+      <c r="X13" s="94"/>
+      <c r="Y13" s="94"/>
+      <c r="Z13" s="78"/>
+      <c r="AA13" s="85"/>
+      <c r="AB13" s="86"/>
     </row>
     <row r="14" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="41">
+      <c r="A14" s="95">
         <v>2</v>
       </c>
-      <c r="B14" s="62"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="64" t="s">
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="65"/>
+      <c r="H14" s="100"/>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="38"/>
+      <c r="L14" s="83"/>
+      <c r="M14" s="98"/>
+      <c r="N14" s="84"/>
+      <c r="O14" s="83"/>
+      <c r="P14" s="84"/>
       <c r="Q14" s="15"/>
-      <c r="R14" s="36"/>
-      <c r="S14" s="37"/>
-      <c r="T14" s="38"/>
-      <c r="U14" s="36"/>
-      <c r="V14" s="38"/>
-      <c r="W14" s="36"/>
-      <c r="X14" s="38"/>
-      <c r="Y14" s="36"/>
-      <c r="Z14" s="38"/>
-      <c r="AA14" s="51"/>
-      <c r="AB14" s="60"/>
+      <c r="R14" s="83"/>
+      <c r="S14" s="98"/>
+      <c r="T14" s="84"/>
+      <c r="U14" s="83"/>
+      <c r="V14" s="84"/>
+      <c r="W14" s="83"/>
+      <c r="X14" s="84"/>
+      <c r="Y14" s="83"/>
+      <c r="Z14" s="84"/>
+      <c r="AA14" s="85"/>
+      <c r="AB14" s="86"/>
     </row>
     <row r="15" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="61"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="64" t="s">
+      <c r="A15" s="96"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="99" t="s">
         <v>70</v>
       </c>
-      <c r="H15" s="65"/>
+      <c r="H15" s="100"/>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="38"/>
+      <c r="L15" s="83"/>
+      <c r="M15" s="98"/>
+      <c r="N15" s="84"/>
+      <c r="O15" s="83"/>
+      <c r="P15" s="84"/>
       <c r="Q15" s="15"/>
-      <c r="R15" s="36"/>
-      <c r="S15" s="37"/>
-      <c r="T15" s="38"/>
-      <c r="U15" s="36"/>
-      <c r="V15" s="38"/>
-      <c r="W15" s="36"/>
-      <c r="X15" s="38"/>
-      <c r="Y15" s="36"/>
-      <c r="Z15" s="38"/>
-      <c r="AA15" s="51"/>
-      <c r="AB15" s="60"/>
+      <c r="R15" s="83"/>
+      <c r="S15" s="98"/>
+      <c r="T15" s="84"/>
+      <c r="U15" s="83"/>
+      <c r="V15" s="84"/>
+      <c r="W15" s="83"/>
+      <c r="X15" s="84"/>
+      <c r="Y15" s="83"/>
+      <c r="Z15" s="84"/>
+      <c r="AA15" s="85"/>
+      <c r="AB15" s="86"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A16" s="61"/>
-      <c r="B16" s="30" t="s">
+      <c r="A16" s="96"/>
+      <c r="B16" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="32"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="93"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="93"/>
+      <c r="K16" s="93"/>
+      <c r="L16" s="76"/>
       <c r="M16" s="20"/>
       <c r="N16" s="21"/>
       <c r="O16" s="18"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="21"/>
       <c r="R16" s="18"/>
-      <c r="S16" s="30"/>
-      <c r="T16" s="32"/>
-      <c r="U16" s="30"/>
-      <c r="V16" s="31"/>
-      <c r="W16" s="31"/>
-      <c r="X16" s="31"/>
-      <c r="Y16" s="31"/>
-      <c r="Z16" s="32"/>
-      <c r="AA16" s="51"/>
-      <c r="AB16" s="60"/>
+      <c r="S16" s="75"/>
+      <c r="T16" s="76"/>
+      <c r="U16" s="75"/>
+      <c r="V16" s="93"/>
+      <c r="W16" s="93"/>
+      <c r="X16" s="93"/>
+      <c r="Y16" s="93"/>
+      <c r="Z16" s="76"/>
+      <c r="AA16" s="85"/>
+      <c r="AB16" s="86"/>
     </row>
     <row r="17" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="42"/>
-      <c r="B17" s="33" t="s">
+      <c r="A17" s="97"/>
+      <c r="B17" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="35"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="94"/>
+      <c r="E17" s="94"/>
+      <c r="F17" s="94"/>
+      <c r="G17" s="94"/>
+      <c r="H17" s="94"/>
+      <c r="I17" s="94"/>
+      <c r="J17" s="94"/>
+      <c r="K17" s="94"/>
+      <c r="L17" s="78"/>
       <c r="M17" s="16"/>
       <c r="N17" s="9"/>
       <c r="O17" s="15"/>
       <c r="P17" s="16"/>
       <c r="Q17" s="9"/>
       <c r="R17" s="15"/>
-      <c r="S17" s="33"/>
-      <c r="T17" s="35"/>
-      <c r="U17" s="33"/>
-      <c r="V17" s="34"/>
-      <c r="W17" s="34"/>
-      <c r="X17" s="34"/>
-      <c r="Y17" s="34"/>
-      <c r="Z17" s="35"/>
-      <c r="AA17" s="51"/>
-      <c r="AB17" s="60"/>
+      <c r="S17" s="77"/>
+      <c r="T17" s="78"/>
+      <c r="U17" s="77"/>
+      <c r="V17" s="94"/>
+      <c r="W17" s="94"/>
+      <c r="X17" s="94"/>
+      <c r="Y17" s="94"/>
+      <c r="Z17" s="78"/>
+      <c r="AA17" s="85"/>
+      <c r="AB17" s="86"/>
     </row>
     <row r="18" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="62"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="39" t="s">
+      <c r="B18" s="73"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="40"/>
+      <c r="H18" s="39"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="38"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="38"/>
+      <c r="L18" s="83"/>
+      <c r="M18" s="98"/>
+      <c r="N18" s="84"/>
+      <c r="O18" s="83"/>
+      <c r="P18" s="84"/>
       <c r="Q18" s="15"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="37"/>
-      <c r="T18" s="38"/>
-      <c r="U18" s="36"/>
-      <c r="V18" s="38"/>
-      <c r="W18" s="36"/>
-      <c r="X18" s="38"/>
-      <c r="Y18" s="36"/>
-      <c r="Z18" s="38"/>
-      <c r="AA18" s="51"/>
-      <c r="AB18" s="60"/>
+      <c r="R18" s="83"/>
+      <c r="S18" s="98"/>
+      <c r="T18" s="84"/>
+      <c r="U18" s="83"/>
+      <c r="V18" s="84"/>
+      <c r="W18" s="83"/>
+      <c r="X18" s="84"/>
+      <c r="Y18" s="83"/>
+      <c r="Z18" s="84"/>
+      <c r="AA18" s="85"/>
+      <c r="AB18" s="86"/>
     </row>
     <row r="19" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="61"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="39" t="s">
+      <c r="A19" s="96"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="74"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="H19" s="40"/>
+      <c r="H19" s="39"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="38"/>
+      <c r="L19" s="83"/>
+      <c r="M19" s="98"/>
+      <c r="N19" s="84"/>
+      <c r="O19" s="83"/>
+      <c r="P19" s="84"/>
       <c r="Q19" s="15"/>
-      <c r="R19" s="36"/>
-      <c r="S19" s="37"/>
-      <c r="T19" s="38"/>
-      <c r="U19" s="36"/>
-      <c r="V19" s="38"/>
-      <c r="W19" s="36"/>
-      <c r="X19" s="38"/>
-      <c r="Y19" s="36"/>
-      <c r="Z19" s="38"/>
-      <c r="AA19" s="51"/>
-      <c r="AB19" s="60"/>
+      <c r="R19" s="83"/>
+      <c r="S19" s="98"/>
+      <c r="T19" s="84"/>
+      <c r="U19" s="83"/>
+      <c r="V19" s="84"/>
+      <c r="W19" s="83"/>
+      <c r="X19" s="84"/>
+      <c r="Y19" s="83"/>
+      <c r="Z19" s="84"/>
+      <c r="AA19" s="85"/>
+      <c r="AB19" s="86"/>
     </row>
     <row r="20" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="61"/>
-      <c r="B20" s="68" t="s">
+      <c r="A20" s="96"/>
+      <c r="B20" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="70"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="66"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="44"/>
-      <c r="P20" s="45"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="82"/>
+      <c r="L20" s="58"/>
+      <c r="M20" s="59"/>
+      <c r="N20" s="60"/>
+      <c r="O20" s="58"/>
+      <c r="P20" s="60"/>
       <c r="Q20" s="21"/>
-      <c r="R20" s="44"/>
-      <c r="S20" s="66"/>
-      <c r="T20" s="45"/>
-      <c r="U20" s="30"/>
-      <c r="V20" s="31"/>
-      <c r="W20" s="31"/>
-      <c r="X20" s="31"/>
-      <c r="Y20" s="31"/>
-      <c r="Z20" s="32"/>
-      <c r="AA20" s="51"/>
-      <c r="AB20" s="60"/>
+      <c r="R20" s="58"/>
+      <c r="S20" s="59"/>
+      <c r="T20" s="60"/>
+      <c r="U20" s="75"/>
+      <c r="V20" s="93"/>
+      <c r="W20" s="93"/>
+      <c r="X20" s="93"/>
+      <c r="Y20" s="93"/>
+      <c r="Z20" s="76"/>
+      <c r="AA20" s="85"/>
+      <c r="AB20" s="86"/>
     </row>
     <row r="21" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="42"/>
-      <c r="B21" s="77" t="s">
+      <c r="A21" s="97"/>
+      <c r="B21" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="78"/>
-      <c r="D21" s="78"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="78"/>
-      <c r="J21" s="78"/>
-      <c r="K21" s="79"/>
-      <c r="L21" s="46"/>
-      <c r="M21" s="67"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="46"/>
-      <c r="P21" s="47"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="65"/>
+      <c r="N21" s="66"/>
+      <c r="O21" s="64"/>
+      <c r="P21" s="66"/>
       <c r="Q21" s="9"/>
-      <c r="R21" s="46"/>
-      <c r="S21" s="67"/>
-      <c r="T21" s="47"/>
-      <c r="U21" s="33"/>
-      <c r="V21" s="34"/>
-      <c r="W21" s="34"/>
-      <c r="X21" s="34"/>
-      <c r="Y21" s="34"/>
-      <c r="Z21" s="35"/>
-      <c r="AA21" s="51"/>
-      <c r="AB21" s="60"/>
+      <c r="R21" s="64"/>
+      <c r="S21" s="65"/>
+      <c r="T21" s="66"/>
+      <c r="U21" s="77"/>
+      <c r="V21" s="94"/>
+      <c r="W21" s="94"/>
+      <c r="X21" s="94"/>
+      <c r="Y21" s="94"/>
+      <c r="Z21" s="78"/>
+      <c r="AA21" s="85"/>
+      <c r="AB21" s="86"/>
     </row>
     <row r="22" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="41">
+      <c r="A22" s="95">
         <v>500</v>
       </c>
-      <c r="B22" s="62"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="39" t="s">
+      <c r="B22" s="73"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="H22" s="40"/>
+      <c r="H22" s="39"/>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="38"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="38"/>
+      <c r="L22" s="83"/>
+      <c r="M22" s="98"/>
+      <c r="N22" s="84"/>
+      <c r="O22" s="83"/>
+      <c r="P22" s="84"/>
       <c r="Q22" s="15"/>
-      <c r="R22" s="36"/>
-      <c r="S22" s="37"/>
-      <c r="T22" s="38"/>
-      <c r="U22" s="36"/>
-      <c r="V22" s="38"/>
-      <c r="W22" s="36"/>
-      <c r="X22" s="38"/>
-      <c r="Y22" s="36"/>
-      <c r="Z22" s="38"/>
-      <c r="AA22" s="51"/>
-      <c r="AB22" s="60"/>
+      <c r="R22" s="83"/>
+      <c r="S22" s="98"/>
+      <c r="T22" s="84"/>
+      <c r="U22" s="83"/>
+      <c r="V22" s="84"/>
+      <c r="W22" s="83"/>
+      <c r="X22" s="84"/>
+      <c r="Y22" s="83"/>
+      <c r="Z22" s="84"/>
+      <c r="AA22" s="85"/>
+      <c r="AB22" s="86"/>
     </row>
     <row r="23" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="61"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="39" t="s">
+      <c r="A23" s="96"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="H23" s="40"/>
+      <c r="H23" s="39"/>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="38"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="38"/>
+      <c r="L23" s="83"/>
+      <c r="M23" s="98"/>
+      <c r="N23" s="84"/>
+      <c r="O23" s="83"/>
+      <c r="P23" s="84"/>
       <c r="Q23" s="15"/>
-      <c r="R23" s="36"/>
-      <c r="S23" s="37"/>
-      <c r="T23" s="38"/>
-      <c r="U23" s="36"/>
-      <c r="V23" s="38"/>
-      <c r="W23" s="36"/>
-      <c r="X23" s="38"/>
-      <c r="Y23" s="36"/>
-      <c r="Z23" s="38"/>
-      <c r="AA23" s="51"/>
-      <c r="AB23" s="60"/>
+      <c r="R23" s="83"/>
+      <c r="S23" s="98"/>
+      <c r="T23" s="84"/>
+      <c r="U23" s="83"/>
+      <c r="V23" s="84"/>
+      <c r="W23" s="83"/>
+      <c r="X23" s="84"/>
+      <c r="Y23" s="83"/>
+      <c r="Z23" s="84"/>
+      <c r="AA23" s="85"/>
+      <c r="AB23" s="86"/>
     </row>
     <row r="24" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="61"/>
-      <c r="B24" s="68" t="s">
+      <c r="A24" s="96"/>
+      <c r="B24" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="69"/>
-      <c r="J24" s="69"/>
-      <c r="K24" s="70"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="66"/>
-      <c r="N24" s="45"/>
-      <c r="O24" s="44"/>
-      <c r="P24" s="45"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="81"/>
+      <c r="J24" s="81"/>
+      <c r="K24" s="82"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="59"/>
+      <c r="N24" s="60"/>
+      <c r="O24" s="58"/>
+      <c r="P24" s="60"/>
       <c r="Q24" s="21"/>
-      <c r="R24" s="44"/>
-      <c r="S24" s="66"/>
-      <c r="T24" s="45"/>
-      <c r="U24" s="30"/>
-      <c r="V24" s="31"/>
-      <c r="W24" s="31"/>
-      <c r="X24" s="31"/>
-      <c r="Y24" s="31"/>
-      <c r="Z24" s="32"/>
-      <c r="AA24" s="51"/>
-      <c r="AB24" s="60"/>
+      <c r="R24" s="58"/>
+      <c r="S24" s="59"/>
+      <c r="T24" s="60"/>
+      <c r="U24" s="75"/>
+      <c r="V24" s="93"/>
+      <c r="W24" s="93"/>
+      <c r="X24" s="93"/>
+      <c r="Y24" s="93"/>
+      <c r="Z24" s="76"/>
+      <c r="AA24" s="85"/>
+      <c r="AB24" s="86"/>
     </row>
     <row r="25" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="42"/>
-      <c r="B25" s="77" t="s">
+      <c r="A25" s="97"/>
+      <c r="B25" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="78"/>
-      <c r="D25" s="78"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="78"/>
-      <c r="H25" s="78"/>
-      <c r="I25" s="78"/>
-      <c r="J25" s="78"/>
-      <c r="K25" s="79"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="67"/>
-      <c r="N25" s="47"/>
-      <c r="O25" s="46"/>
-      <c r="P25" s="47"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="65"/>
+      <c r="N25" s="66"/>
+      <c r="O25" s="64"/>
+      <c r="P25" s="66"/>
       <c r="Q25" s="9"/>
-      <c r="R25" s="46"/>
-      <c r="S25" s="67"/>
-      <c r="T25" s="47"/>
-      <c r="U25" s="33"/>
-      <c r="V25" s="34"/>
-      <c r="W25" s="34"/>
-      <c r="X25" s="34"/>
-      <c r="Y25" s="34"/>
-      <c r="Z25" s="35"/>
-      <c r="AA25" s="51"/>
-      <c r="AB25" s="60"/>
+      <c r="R25" s="64"/>
+      <c r="S25" s="65"/>
+      <c r="T25" s="66"/>
+      <c r="U25" s="77"/>
+      <c r="V25" s="94"/>
+      <c r="W25" s="94"/>
+      <c r="X25" s="94"/>
+      <c r="Y25" s="94"/>
+      <c r="Z25" s="78"/>
+      <c r="AA25" s="85"/>
+      <c r="AB25" s="86"/>
     </row>
     <row r="26" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="68" t="s">
+      <c r="A26" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="69"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="69"/>
-      <c r="I26" s="69"/>
-      <c r="J26" s="69"/>
-      <c r="K26" s="70"/>
-      <c r="L26" s="44"/>
-      <c r="M26" s="66"/>
-      <c r="N26" s="45"/>
+      <c r="B26" s="81"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="81"/>
+      <c r="F26" s="81"/>
+      <c r="G26" s="81"/>
+      <c r="H26" s="81"/>
+      <c r="I26" s="81"/>
+      <c r="J26" s="81"/>
+      <c r="K26" s="82"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="59"/>
+      <c r="N26" s="60"/>
       <c r="O26" s="20"/>
       <c r="P26" s="21"/>
       <c r="Q26" s="21"/>
-      <c r="R26" s="44"/>
-      <c r="S26" s="66"/>
-      <c r="T26" s="45"/>
-      <c r="U26" s="56"/>
-      <c r="V26" s="74"/>
-      <c r="W26" s="74"/>
-      <c r="X26" s="74"/>
-      <c r="Y26" s="74"/>
-      <c r="Z26" s="57"/>
-      <c r="AA26" s="51"/>
-      <c r="AB26" s="60"/>
+      <c r="R26" s="58"/>
+      <c r="S26" s="59"/>
+      <c r="T26" s="60"/>
+      <c r="U26" s="87"/>
+      <c r="V26" s="88"/>
+      <c r="W26" s="88"/>
+      <c r="X26" s="88"/>
+      <c r="Y26" s="88"/>
+      <c r="Z26" s="89"/>
+      <c r="AA26" s="85"/>
+      <c r="AB26" s="86"/>
     </row>
     <row r="27" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="78"/>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="78"/>
-      <c r="I27" s="78"/>
-      <c r="J27" s="78"/>
-      <c r="K27" s="79"/>
-      <c r="L27" s="46"/>
-      <c r="M27" s="67"/>
-      <c r="N27" s="47"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="65"/>
+      <c r="N27" s="66"/>
       <c r="O27" s="16"/>
       <c r="P27" s="9"/>
       <c r="Q27" s="9"/>
-      <c r="R27" s="46"/>
-      <c r="S27" s="67"/>
-      <c r="T27" s="47"/>
-      <c r="U27" s="58"/>
-      <c r="V27" s="75"/>
-      <c r="W27" s="75"/>
-      <c r="X27" s="75"/>
-      <c r="Y27" s="75"/>
-      <c r="Z27" s="59"/>
-      <c r="AA27" s="51"/>
-      <c r="AB27" s="60"/>
+      <c r="R27" s="64"/>
+      <c r="S27" s="65"/>
+      <c r="T27" s="66"/>
+      <c r="U27" s="90"/>
+      <c r="V27" s="91"/>
+      <c r="W27" s="91"/>
+      <c r="X27" s="91"/>
+      <c r="Y27" s="91"/>
+      <c r="Z27" s="92"/>
+      <c r="AA27" s="85"/>
+      <c r="AB27" s="86"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
@@ -7819,36 +7819,36 @@
       <c r="A29" s="17"/>
     </row>
     <row r="30" spans="1:28" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="81" t="s">
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="K30" s="82"/>
-      <c r="L30" s="83"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="45"/>
     </row>
     <row r="31" spans="1:28" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="43"/>
-      <c r="C31" s="40"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
       <c r="D31" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="39" t="s">
+      <c r="E31" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="F31" s="40"/>
+      <c r="F31" s="39"/>
       <c r="G31" s="25" t="s">
         <v>46</v>
       </c>
@@ -7858,23 +7858,23 @@
       <c r="I31" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="J31" s="84"/>
-      <c r="K31" s="85"/>
-      <c r="L31" s="86"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="48"/>
     </row>
     <row r="32" spans="1:28" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="48" t="s">
+      <c r="A32" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="50"/>
-      <c r="C32" s="49"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="42"/>
       <c r="D32" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="F32" s="49"/>
+      <c r="F32" s="42"/>
       <c r="G32" s="14" t="s">
         <v>52</v>
       </c>
@@ -7884,207 +7884,207 @@
       <c r="I32" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="J32" s="99">
+      <c r="J32" s="67">
         <v>14</v>
       </c>
-      <c r="K32" s="100"/>
-      <c r="L32" s="101"/>
+      <c r="K32" s="68"/>
+      <c r="L32" s="69"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="39"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="40"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="39"/>
       <c r="D33" s="15"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="40"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
-      <c r="J33" s="99"/>
-      <c r="K33" s="100"/>
-      <c r="L33" s="101"/>
+      <c r="J33" s="67"/>
+      <c r="K33" s="68"/>
+      <c r="L33" s="69"/>
     </row>
     <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="39"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="40"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="39"/>
       <c r="D34" s="15"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="40"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
-      <c r="J34" s="99"/>
-      <c r="K34" s="100"/>
-      <c r="L34" s="101"/>
+      <c r="J34" s="67"/>
+      <c r="K34" s="68"/>
+      <c r="L34" s="69"/>
     </row>
     <row r="35" spans="1:12" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="71" t="s">
+      <c r="A35" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="72"/>
-      <c r="C35" s="73"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="15"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="40"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
-      <c r="J35" s="99"/>
-      <c r="K35" s="100"/>
-      <c r="L35" s="101"/>
+      <c r="J35" s="67"/>
+      <c r="K35" s="68"/>
+      <c r="L35" s="69"/>
     </row>
     <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="71"/>
-      <c r="B36" s="72"/>
-      <c r="C36" s="73"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="32"/>
       <c r="D36" s="15"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="40"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
       <c r="I36" s="15"/>
-      <c r="J36" s="99"/>
-      <c r="K36" s="100"/>
-      <c r="L36" s="101"/>
+      <c r="J36" s="67"/>
+      <c r="K36" s="68"/>
+      <c r="L36" s="69"/>
     </row>
     <row r="37" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="71"/>
-      <c r="B37" s="72"/>
-      <c r="C37" s="73"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="32"/>
       <c r="D37" s="15"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="40"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
       <c r="I37" s="15"/>
-      <c r="J37" s="102"/>
-      <c r="K37" s="103"/>
-      <c r="L37" s="104"/>
+      <c r="J37" s="70"/>
+      <c r="K37" s="71"/>
+      <c r="L37" s="72"/>
     </row>
     <row r="38" spans="1:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="71" t="s">
+      <c r="A38" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="72"/>
-      <c r="C38" s="73"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="32"/>
       <c r="D38" s="15"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="40"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="39"/>
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>
-      <c r="J38" s="87" t="s">
+      <c r="J38" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="K38" s="88"/>
-      <c r="L38" s="89"/>
+      <c r="K38" s="50"/>
+      <c r="L38" s="51"/>
     </row>
     <row r="39" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="71"/>
-      <c r="B39" s="72"/>
-      <c r="C39" s="73"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="32"/>
       <c r="D39" s="15"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="40"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="39"/>
       <c r="G39" s="15"/>
       <c r="H39" s="15"/>
       <c r="I39" s="15"/>
-      <c r="J39" s="90"/>
-      <c r="K39" s="91"/>
-      <c r="L39" s="92"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="53"/>
+      <c r="L39" s="54"/>
     </row>
     <row r="40" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="71"/>
-      <c r="B40" s="72"/>
-      <c r="C40" s="73"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="32"/>
       <c r="D40" s="15"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="40"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="39"/>
       <c r="G40" s="15"/>
       <c r="H40" s="15"/>
       <c r="I40" s="15"/>
-      <c r="J40" s="90"/>
-      <c r="K40" s="91"/>
-      <c r="L40" s="92"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="53"/>
+      <c r="L40" s="54"/>
     </row>
     <row r="41" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="71" t="s">
+      <c r="A41" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="72"/>
-      <c r="C41" s="73"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="32"/>
       <c r="D41" s="15"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="40"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="39"/>
       <c r="G41" s="15"/>
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
-      <c r="J41" s="90"/>
-      <c r="K41" s="91"/>
-      <c r="L41" s="92"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="53"/>
+      <c r="L41" s="54"/>
     </row>
     <row r="42" spans="1:12" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="71" t="s">
+      <c r="A42" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="72"/>
-      <c r="C42" s="73"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="32"/>
       <c r="D42" s="15"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="40"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="39"/>
       <c r="G42" s="15"/>
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
-      <c r="J42" s="93"/>
-      <c r="K42" s="94"/>
-      <c r="L42" s="95"/>
+      <c r="J42" s="55"/>
+      <c r="K42" s="56"/>
+      <c r="L42" s="57"/>
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="44" t="s">
+      <c r="A43" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="66"/>
-      <c r="C43" s="66"/>
-      <c r="D43" s="66"/>
-      <c r="E43" s="66"/>
-      <c r="F43" s="66"/>
-      <c r="G43" s="66"/>
-      <c r="H43" s="66"/>
-      <c r="I43" s="45"/>
-      <c r="J43" s="87" t="s">
+      <c r="B43" s="59"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="59"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="59"/>
+      <c r="H43" s="59"/>
+      <c r="I43" s="60"/>
+      <c r="J43" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="K43" s="88"/>
-      <c r="L43" s="89"/>
+      <c r="K43" s="50"/>
+      <c r="L43" s="51"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="96"/>
-      <c r="B44" s="97"/>
-      <c r="C44" s="97"/>
-      <c r="D44" s="97"/>
-      <c r="E44" s="97"/>
-      <c r="F44" s="97"/>
-      <c r="G44" s="97"/>
-      <c r="H44" s="97"/>
-      <c r="I44" s="98"/>
-      <c r="J44" s="90"/>
-      <c r="K44" s="91"/>
-      <c r="L44" s="92"/>
+      <c r="A44" s="61"/>
+      <c r="B44" s="62"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="62"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="62"/>
+      <c r="I44" s="63"/>
+      <c r="J44" s="52"/>
+      <c r="K44" s="53"/>
+      <c r="L44" s="54"/>
     </row>
     <row r="45" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="46"/>
-      <c r="B45" s="67"/>
-      <c r="C45" s="67"/>
-      <c r="D45" s="67"/>
-      <c r="E45" s="67"/>
-      <c r="F45" s="67"/>
-      <c r="G45" s="67"/>
-      <c r="H45" s="67"/>
-      <c r="I45" s="47"/>
-      <c r="J45" s="93"/>
-      <c r="K45" s="94"/>
-      <c r="L45" s="95"/>
+      <c r="A45" s="64"/>
+      <c r="B45" s="65"/>
+      <c r="C45" s="65"/>
+      <c r="D45" s="65"/>
+      <c r="E45" s="65"/>
+      <c r="F45" s="65"/>
+      <c r="G45" s="65"/>
+      <c r="H45" s="65"/>
+      <c r="I45" s="66"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="56"/>
+      <c r="L45" s="57"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="19"/>
@@ -8095,33 +8095,204 @@
       </c>
     </row>
     <row r="48" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="80" t="s">
+      <c r="A48" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="B48" s="80"/>
-      <c r="C48" s="80"/>
-      <c r="D48" s="80"/>
-      <c r="E48" s="80"/>
-      <c r="F48" s="80"/>
-      <c r="G48" s="80"/>
-      <c r="H48" s="80"/>
-      <c r="I48" s="80"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="36"/>
     </row>
     <row r="49" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="80" t="s">
+      <c r="A49" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="B49" s="80"/>
-      <c r="C49" s="80"/>
-      <c r="D49" s="80"/>
-      <c r="E49" s="80"/>
-      <c r="F49" s="80"/>
-      <c r="G49" s="80"/>
-      <c r="H49" s="80"/>
-      <c r="I49" s="80"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="36"/>
+      <c r="I49" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="195">
+    <mergeCell ref="A4:E5"/>
+    <mergeCell ref="F4:I5"/>
+    <mergeCell ref="J4:S4"/>
+    <mergeCell ref="J5:S5"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:F8"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Y8:Z9"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:F11"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O12:P13"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="AA14:AB14"/>
+    <mergeCell ref="R12:T13"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="W18:X18"/>
+    <mergeCell ref="AA16:AB17"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="S16:T17"/>
+    <mergeCell ref="U16:Z17"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="U12:Z13"/>
+    <mergeCell ref="AA12:AB13"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="Y18:Z18"/>
+    <mergeCell ref="AA18:AB18"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="B16:L16"/>
+    <mergeCell ref="B17:L17"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="W14:X14"/>
+    <mergeCell ref="Y14:Z14"/>
+    <mergeCell ref="AA22:AB22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="W19:X19"/>
+    <mergeCell ref="Y19:Z19"/>
+    <mergeCell ref="AA19:AB19"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="U20:Z21"/>
+    <mergeCell ref="R20:T21"/>
+    <mergeCell ref="O20:P21"/>
+    <mergeCell ref="L20:N21"/>
+    <mergeCell ref="B20:K20"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="Y22:Z22"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="G6:T6"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="AA26:AB27"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="U26:Z27"/>
+    <mergeCell ref="Y23:Z23"/>
+    <mergeCell ref="AA23:AB23"/>
+    <mergeCell ref="U24:Z25"/>
+    <mergeCell ref="AA24:AB25"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="AA20:AB21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:F23"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A2:Z2"/>
+    <mergeCell ref="A1:Z1"/>
+    <mergeCell ref="A26:K26"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="L26:N27"/>
+    <mergeCell ref="R26:T27"/>
+    <mergeCell ref="R24:T25"/>
+    <mergeCell ref="T4:X4"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="A3:Z3"/>
+    <mergeCell ref="O24:P25"/>
+    <mergeCell ref="L24:N25"/>
+    <mergeCell ref="B24:K24"/>
+    <mergeCell ref="B25:K25"/>
+    <mergeCell ref="U6:X6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="B13:K13"/>
+    <mergeCell ref="L12:N13"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="B21:K21"/>
@@ -8146,177 +8317,6 @@
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="E40:F40"/>
     <mergeCell ref="E41:F41"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:F23"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A2:Z2"/>
-    <mergeCell ref="A1:Z1"/>
-    <mergeCell ref="A26:K26"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="L26:N27"/>
-    <mergeCell ref="R26:T27"/>
-    <mergeCell ref="R24:T25"/>
-    <mergeCell ref="T4:X4"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="A3:Z3"/>
-    <mergeCell ref="O24:P25"/>
-    <mergeCell ref="L24:N25"/>
-    <mergeCell ref="B24:K24"/>
-    <mergeCell ref="B25:K25"/>
-    <mergeCell ref="U6:X6"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="B12:K12"/>
-    <mergeCell ref="B13:K13"/>
-    <mergeCell ref="L12:N13"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="Y22:Z22"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="G6:T6"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="AA26:AB27"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="U26:Z27"/>
-    <mergeCell ref="Y23:Z23"/>
-    <mergeCell ref="AA23:AB23"/>
-    <mergeCell ref="U24:Z25"/>
-    <mergeCell ref="AA24:AB25"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="AA20:AB21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="AA22:AB22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="L23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="W19:X19"/>
-    <mergeCell ref="Y19:Z19"/>
-    <mergeCell ref="AA19:AB19"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="U20:Z21"/>
-    <mergeCell ref="R20:T21"/>
-    <mergeCell ref="O20:P21"/>
-    <mergeCell ref="L20:N21"/>
-    <mergeCell ref="B20:K20"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="Y18:Z18"/>
-    <mergeCell ref="AA18:AB18"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="B16:L16"/>
-    <mergeCell ref="B17:L17"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="AA15:AB15"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="R14:T14"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="W14:X14"/>
-    <mergeCell ref="Y14:Z14"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="W18:X18"/>
-    <mergeCell ref="AA16:AB17"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="W11:X11"/>
-    <mergeCell ref="Y11:Z11"/>
-    <mergeCell ref="S16:T17"/>
-    <mergeCell ref="U16:Z17"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="U12:Z13"/>
-    <mergeCell ref="AA12:AB13"/>
-    <mergeCell ref="R15:T15"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="W15:X15"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="AA14:AB14"/>
-    <mergeCell ref="R12:T13"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:F11"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O12:P13"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="Y8:Z9"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="A4:E5"/>
-    <mergeCell ref="F4:I5"/>
-    <mergeCell ref="J4:S4"/>
-    <mergeCell ref="J5:S5"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:P7"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:F8"/>
-    <mergeCell ref="G7:H8"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="Y7:Z7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>